<commit_message>
Removed moonsharp error bypass
</commit_message>
<xml_diff>
--- a/ColorizedResults.xlsx
+++ b/ColorizedResults.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Znnin\Documents\Visual Studio 2019\Projects\LuaDotNetPerfExploration\PerfTester\bin\Debug\net5.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5D0DEC12-E61A-4819-84AD-322B4CC43B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637A775A-7A99-442E-B7C4-45B1929CE62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39285" yWindow="-120" windowWidth="37635" windowHeight="21840"/>
+    <workbookView xWindow="45345" yWindow="5820" windowWidth="28050" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1089,11 +1089,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="B2" sqref="B2:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,37 +1165,37 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="D2" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G2" s="1">
-        <v>2352</v>
+        <v>2325</v>
       </c>
       <c r="H2" s="3">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I2" s="2">
-        <v>730</v>
+        <v>747</v>
       </c>
       <c r="J2" s="1">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="K2" s="1">
-        <v>247</v>
+        <v>438</v>
       </c>
       <c r="L2" s="1">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="M2" s="3">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N2" t="s">
         <v>13</v>
@@ -1206,40 +1206,40 @@
         <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D3" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F3" s="2">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G3" s="1">
-        <v>2528</v>
+        <v>2536</v>
       </c>
       <c r="H3" s="3">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2">
-        <v>565</v>
+        <v>585</v>
       </c>
       <c r="J3" s="1">
-        <v>1100</v>
+        <v>1113</v>
       </c>
       <c r="K3" s="1">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L3" s="1">
         <v>125</v>
       </c>
       <c r="M3" s="3">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="N3" t="s">
         <v>13</v>
@@ -1253,37 +1253,37 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="D4" s="1">
         <v>15</v>
       </c>
       <c r="E4" s="3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="G4" s="1">
-        <v>2363</v>
+        <v>2316</v>
       </c>
       <c r="H4" s="3">
         <v>77</v>
       </c>
       <c r="I4" s="2">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J4" s="1">
-        <v>1085</v>
+        <v>1096</v>
       </c>
       <c r="K4" s="1">
         <v>142</v>
       </c>
       <c r="L4" s="1">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M4" s="3">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N4" t="s">
         <v>13</v>
@@ -1297,37 +1297,37 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D5" s="1">
         <v>17</v>
       </c>
       <c r="E5" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="G5" s="1">
-        <v>2408</v>
+        <v>2539</v>
       </c>
       <c r="H5" s="3">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I5" s="2">
-        <v>551</v>
+        <v>565</v>
       </c>
       <c r="J5" s="1">
-        <v>1092</v>
+        <v>1099</v>
       </c>
       <c r="K5" s="1">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L5" s="1">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="M5" s="3">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="N5" t="s">
         <v>13</v>
@@ -1341,37 +1341,37 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="D6" s="1">
         <v>15</v>
       </c>
       <c r="E6" s="3">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2">
         <v>374</v>
       </c>
       <c r="G6" s="1">
-        <v>2492</v>
+        <v>2301</v>
       </c>
       <c r="H6" s="3">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I6" s="2">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="J6" s="1">
-        <v>1088</v>
+        <v>1118</v>
       </c>
       <c r="K6" s="1">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L6" s="1">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M6" s="3">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N6" t="s">
         <v>13</v>
@@ -1385,37 +1385,37 @@
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D7" s="1">
         <v>17</v>
       </c>
       <c r="E7" s="3">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="G7" s="1">
-        <v>2473</v>
+        <v>2458</v>
       </c>
       <c r="H7" s="3">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I7" s="2">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="J7" s="1">
-        <v>1104</v>
+        <v>1095</v>
       </c>
       <c r="K7" s="1">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L7" s="1">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="M7" s="3">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="N7" t="s">
         <v>13</v>
@@ -1429,7 +1429,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="D8" s="1">
         <v>16</v>
@@ -1438,28 +1438,28 @@
         <v>92</v>
       </c>
       <c r="F8" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="G8" s="1">
-        <v>2656</v>
+        <v>2471</v>
       </c>
       <c r="H8" s="3">
         <v>79</v>
       </c>
       <c r="I8" s="2">
-        <v>528</v>
+        <v>588</v>
       </c>
       <c r="J8" s="1">
-        <v>1064</v>
+        <v>1085</v>
       </c>
       <c r="K8" s="1">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L8" s="1">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="M8" s="3">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N8" t="s">
         <v>13</v>
@@ -1470,40 +1470,40 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D9" s="1">
         <v>16</v>
       </c>
       <c r="E9" s="3">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="G9" s="1">
-        <v>2623</v>
+        <v>2566</v>
       </c>
       <c r="H9" s="3">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I9" s="2">
-        <v>548</v>
+        <v>696</v>
       </c>
       <c r="J9" s="1">
-        <v>1079</v>
+        <v>1092</v>
       </c>
       <c r="K9" s="1">
+        <v>131</v>
+      </c>
+      <c r="L9" s="1">
+        <v>135</v>
+      </c>
+      <c r="M9" s="3">
         <v>129</v>
-      </c>
-      <c r="L9" s="1">
-        <v>124</v>
-      </c>
-      <c r="M9" s="3">
-        <v>132</v>
       </c>
       <c r="N9" t="s">
         <v>13</v>
@@ -1514,40 +1514,40 @@
         <v>22</v>
       </c>
       <c r="B10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" s="1">
         <v>18</v>
       </c>
       <c r="E10" s="3">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="2">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G10" s="1">
-        <v>2338</v>
+        <v>2303</v>
       </c>
       <c r="H10" s="3">
         <v>80</v>
       </c>
       <c r="I10" s="2">
-        <v>503</v>
+        <v>668</v>
       </c>
       <c r="J10" s="1">
-        <v>1048</v>
+        <v>1056</v>
       </c>
       <c r="K10" s="1">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="L10" s="1">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="M10" s="3">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="N10" t="s">
         <v>13</v>
@@ -1558,40 +1558,40 @@
         <v>23</v>
       </c>
       <c r="B11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D11" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3">
         <v>83</v>
       </c>
       <c r="F11" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="G11" s="1">
-        <v>2393</v>
+        <v>2232</v>
       </c>
       <c r="H11" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I11" s="2">
-        <v>522</v>
+        <v>604</v>
       </c>
       <c r="J11" s="1">
-        <v>1051</v>
+        <v>1071</v>
       </c>
       <c r="K11" s="1">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="L11" s="1">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M11" s="3">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N11" t="s">
         <v>13</v>
@@ -1602,40 +1602,40 @@
         <v>24</v>
       </c>
       <c r="B12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>410</v>
+        <v>381</v>
       </c>
       <c r="D12" s="1">
         <v>18</v>
       </c>
       <c r="E12" s="3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F12" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="G12" s="1">
-        <v>2286</v>
+        <v>2331</v>
       </c>
       <c r="H12" s="3">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I12" s="2">
-        <v>539</v>
+        <v>573</v>
       </c>
       <c r="J12" s="1">
-        <v>1035</v>
+        <v>1053</v>
       </c>
       <c r="K12" s="1">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="L12" s="1">
+        <v>130</v>
+      </c>
+      <c r="M12" s="3">
         <v>133</v>
-      </c>
-      <c r="M12" s="3">
-        <v>132</v>
       </c>
       <c r="N12" t="s">
         <v>13</v>
@@ -1649,37 +1649,37 @@
         <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D13" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F13" s="2">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="G13" s="1">
-        <v>2284</v>
+        <v>2354</v>
       </c>
       <c r="H13" s="3">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I13" s="2">
-        <v>522</v>
+        <v>562</v>
       </c>
       <c r="J13" s="1">
-        <v>1038</v>
+        <v>1062</v>
       </c>
       <c r="K13" s="1">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="L13" s="1">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="M13" s="3">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="N13" t="s">
         <v>13</v>
@@ -1690,40 +1690,40 @@
         <v>26</v>
       </c>
       <c r="B14" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D14" s="1">
         <v>17</v>
       </c>
       <c r="E14" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="G14" s="1">
-        <v>2315</v>
+        <v>2309</v>
       </c>
       <c r="H14" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I14" s="2">
-        <v>502</v>
+        <v>542</v>
       </c>
       <c r="J14" s="1">
-        <v>1047</v>
+        <v>1056</v>
       </c>
       <c r="K14" s="1">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L14" s="1">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="M14" s="3">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="N14" t="s">
         <v>13</v>
@@ -1737,37 +1737,37 @@
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
       </c>
       <c r="E15" s="3">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F15" s="2">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="G15" s="1">
-        <v>2326</v>
+        <v>2312</v>
       </c>
       <c r="H15" s="3">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I15" s="2">
-        <v>520</v>
+        <v>554</v>
       </c>
       <c r="J15" s="1">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="K15" s="1">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L15" s="1">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="M15" s="3">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N15" t="s">
         <v>13</v>
@@ -1781,37 +1781,37 @@
         <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D16" s="1">
         <v>17</v>
       </c>
       <c r="E16" s="3">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F16" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="G16" s="1">
-        <v>2314</v>
+        <v>2333</v>
       </c>
       <c r="H16" s="3">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I16" s="2">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="J16" s="1">
-        <v>1051</v>
+        <v>1059</v>
       </c>
       <c r="K16" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L16" s="1">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M16" s="3">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N16" t="s">
         <v>13</v>
@@ -1825,37 +1825,37 @@
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D17" s="1">
         <v>19</v>
       </c>
       <c r="E17" s="3">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F17" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G17" s="1">
-        <v>2315</v>
+        <v>2238</v>
       </c>
       <c r="H17" s="3">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="2">
-        <v>517</v>
+        <v>547</v>
       </c>
       <c r="J17" s="1">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="K17" s="1">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="L17" s="1">
         <v>135</v>
       </c>
       <c r="M17" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N17" t="s">
         <v>13</v>
@@ -1869,37 +1869,37 @@
         <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D18" s="1">
         <v>17</v>
       </c>
       <c r="E18" s="3">
+        <v>82</v>
+      </c>
+      <c r="F18" s="2">
+        <v>374</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2285</v>
+      </c>
+      <c r="H18" s="3">
         <v>80</v>
       </c>
-      <c r="F18" s="2">
-        <v>377</v>
-      </c>
-      <c r="G18" s="1">
-        <v>2293</v>
-      </c>
-      <c r="H18" s="3">
-        <v>78</v>
-      </c>
       <c r="I18" s="2">
-        <v>500</v>
+        <v>537</v>
       </c>
       <c r="J18" s="1">
-        <v>1064</v>
+        <v>1056</v>
       </c>
       <c r="K18" s="1">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L18" s="1">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="M18" s="3">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="N18" t="s">
         <v>13</v>
@@ -1913,37 +1913,37 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="D19" s="1">
         <v>19</v>
       </c>
       <c r="E19" s="3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F19" s="2">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="G19" s="1">
-        <v>2249</v>
+        <v>2323</v>
       </c>
       <c r="H19" s="3">
         <v>78</v>
       </c>
       <c r="I19" s="2">
-        <v>515</v>
+        <v>534</v>
       </c>
       <c r="J19" s="1">
-        <v>1038</v>
+        <v>1054</v>
       </c>
       <c r="K19" s="1">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="L19" s="1">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M19" s="3">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="N19" t="s">
         <v>13</v>
@@ -1957,34 +1957,34 @@
         <v>2</v>
       </c>
       <c r="C20" s="1">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D20" s="1">
         <v>17</v>
       </c>
       <c r="E20" s="3">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F20" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G20" s="1">
-        <v>2268</v>
+        <v>2278</v>
       </c>
       <c r="H20" s="3">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I20" s="2">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="J20" s="1">
-        <v>1043</v>
+        <v>1069</v>
       </c>
       <c r="K20" s="1">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="L20" s="1">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M20" s="3">
         <v>134</v>
@@ -2001,37 +2001,37 @@
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D21" s="1">
         <v>19</v>
       </c>
       <c r="E21" s="3">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F21" s="2">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="G21" s="1">
-        <v>2280</v>
+        <v>2311</v>
       </c>
       <c r="H21" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I21" s="2">
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="J21" s="1">
-        <v>1036</v>
+        <v>1063</v>
       </c>
       <c r="K21" s="1">
+        <v>140</v>
+      </c>
+      <c r="L21" s="1">
+        <v>140</v>
+      </c>
+      <c r="M21" s="3">
         <v>136</v>
-      </c>
-      <c r="L21" s="1">
-        <v>138</v>
-      </c>
-      <c r="M21" s="3">
-        <v>133</v>
       </c>
       <c r="N21" t="s">
         <v>13</v>
@@ -2045,37 +2045,37 @@
         <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D22" s="1">
         <v>18</v>
       </c>
       <c r="E22" s="3">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F22" s="2">
         <v>388</v>
       </c>
       <c r="G22" s="1">
-        <v>2404</v>
+        <v>2344</v>
       </c>
       <c r="H22" s="3">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I22" s="2">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="J22" s="1">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="K22" s="1">
+        <v>130</v>
+      </c>
+      <c r="L22" s="1">
         <v>131</v>
       </c>
-      <c r="L22" s="1">
-        <v>126</v>
-      </c>
       <c r="M22" s="3">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N22" t="s">
         <v>13</v>
@@ -2086,37 +2086,37 @@
         <v>35</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="D23" s="1">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3">
         <v>135</v>
       </c>
       <c r="F23" s="2">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="G23" s="1">
-        <v>2373</v>
+        <v>2375</v>
       </c>
       <c r="H23" s="3">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I23" s="2">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="J23" s="1">
-        <v>1074</v>
+        <v>1083</v>
       </c>
       <c r="K23" s="1">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="L23" s="1">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="M23" s="3">
         <v>126</v>
@@ -2130,40 +2130,40 @@
         <v>36</v>
       </c>
       <c r="B24" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D24" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F24" s="2">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="G24" s="1">
-        <v>3609</v>
+        <v>3993</v>
       </c>
       <c r="H24" s="3">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I24" s="2">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="J24" s="1">
-        <v>1899</v>
+        <v>1887</v>
       </c>
       <c r="K24" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L24" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M24" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N24" t="s">
         <v>13</v>
@@ -2174,40 +2174,40 @@
         <v>37</v>
       </c>
       <c r="B25" s="2">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D25" s="1">
         <v>36</v>
       </c>
       <c r="E25" s="3">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F25" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G25" s="1">
-        <v>2607</v>
+        <v>2537</v>
       </c>
       <c r="H25" s="3">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I25" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="J25" s="1">
-        <v>1151</v>
+        <v>1142</v>
       </c>
       <c r="K25" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="L25" s="1">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M25" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N25" t="s">
         <v>13</v>
@@ -2221,37 +2221,37 @@
         <v>15</v>
       </c>
       <c r="C26" s="1">
-        <v>2092</v>
+        <v>2119</v>
       </c>
       <c r="D26" s="1">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E26" s="3">
-        <v>5292</v>
+        <v>5274</v>
       </c>
       <c r="F26" s="2">
-        <v>2110</v>
+        <v>2088</v>
       </c>
       <c r="G26" s="1">
-        <v>2601</v>
+        <v>2646</v>
       </c>
       <c r="H26" s="3">
-        <v>5152</v>
+        <v>5205</v>
       </c>
       <c r="I26" s="2">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="J26" s="1">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="K26" s="1">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L26" s="1">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M26" s="3">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N26" t="s">
         <v>13</v>
@@ -2262,40 +2262,40 @@
         <v>39</v>
       </c>
       <c r="B27" s="2">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1">
-        <v>854</v>
+        <v>817</v>
       </c>
       <c r="D27" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E27" s="3">
+        <v>200</v>
+      </c>
+      <c r="F27" s="2">
+        <v>985</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3396</v>
+      </c>
+      <c r="H27" s="3">
         <v>196</v>
       </c>
-      <c r="F27" s="2">
-        <v>1009</v>
-      </c>
-      <c r="G27" s="1">
-        <v>3385</v>
-      </c>
-      <c r="H27" s="3">
-        <v>205</v>
-      </c>
       <c r="I27" s="2">
-        <v>773</v>
+        <v>752</v>
       </c>
       <c r="J27" s="1">
-        <v>2153</v>
+        <v>2174</v>
       </c>
       <c r="K27" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L27" s="1">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="M27" s="3">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N27" t="s">
         <v>13</v>
@@ -2306,40 +2306,40 @@
         <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1">
-        <v>7980</v>
+        <v>8005</v>
       </c>
       <c r="D28" s="1">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="E28" s="3">
-        <v>9507</v>
+        <v>9255</v>
       </c>
       <c r="F28" s="2">
-        <v>8434</v>
+        <v>8179</v>
       </c>
       <c r="G28" s="1">
-        <v>3731</v>
+        <v>3615</v>
       </c>
       <c r="H28" s="3">
-        <v>9582</v>
+        <v>9212</v>
       </c>
       <c r="I28" s="2">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="J28" s="1">
-        <v>2195</v>
+        <v>2211</v>
       </c>
       <c r="K28" s="1">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="L28" s="1">
         <v>123</v>
       </c>
       <c r="M28" s="3">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="N28" t="s">
         <v>13</v>
@@ -2350,40 +2350,40 @@
         <v>41</v>
       </c>
       <c r="B29" s="2">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="C29" s="1">
-        <v>1037</v>
+        <v>1066</v>
       </c>
       <c r="D29" s="1">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E29" s="3">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="F29" s="2">
-        <v>798</v>
+        <v>894</v>
       </c>
       <c r="G29" s="1">
-        <v>2455</v>
+        <v>2573</v>
       </c>
       <c r="H29" s="3">
-        <v>310</v>
+        <v>244</v>
       </c>
       <c r="I29" s="2">
-        <v>845</v>
+        <v>859</v>
       </c>
       <c r="J29" s="1">
-        <v>1361</v>
+        <v>1372</v>
       </c>
       <c r="K29" s="1">
-        <v>409</v>
+        <v>463</v>
       </c>
       <c r="L29" s="1">
-        <v>435</v>
+        <v>371</v>
       </c>
       <c r="M29" s="3">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="N29" t="s">
         <v>13</v>
@@ -2394,40 +2394,40 @@
         <v>42</v>
       </c>
       <c r="B30" s="2">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D30" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="3">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="F30" s="2">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G30" s="1">
-        <v>2578</v>
+        <v>2420</v>
       </c>
       <c r="H30" s="3">
-        <v>148</v>
+        <v>211</v>
       </c>
       <c r="I30" s="2">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="J30" s="1">
-        <v>1033</v>
+        <v>1024</v>
       </c>
       <c r="K30" s="1">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="L30" s="1">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M30" s="3">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="N30" t="s">
         <v>13</v>
@@ -2438,40 +2438,40 @@
         <v>43</v>
       </c>
       <c r="B31" s="2">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1">
-        <v>1130</v>
+        <v>2532416</v>
       </c>
       <c r="D31" s="1">
-        <v>377</v>
+        <v>429</v>
       </c>
       <c r="E31" s="3">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="F31" s="2">
-        <v>1095</v>
+        <v>2644224</v>
       </c>
       <c r="G31" s="1">
-        <v>2323</v>
+        <v>2288</v>
       </c>
       <c r="H31" s="3">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="I31" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="J31" s="1">
-        <v>1281</v>
+        <v>1220</v>
       </c>
       <c r="K31" s="1">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="L31" s="1">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="M31" s="3">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="N31" t="s">
         <v>13</v>
@@ -2482,40 +2482,40 @@
         <v>44</v>
       </c>
       <c r="B32" s="4">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C32" s="5">
-        <v>10529</v>
+        <v>10435</v>
       </c>
       <c r="D32" s="5">
-        <v>946</v>
+        <v>939</v>
       </c>
       <c r="E32" s="6">
-        <v>2355</v>
+        <v>2414</v>
       </c>
       <c r="F32" s="4">
-        <v>10263</v>
+        <v>10102</v>
       </c>
       <c r="G32" s="5">
-        <v>941</v>
+        <v>934</v>
       </c>
       <c r="H32" s="6">
-        <v>2370</v>
+        <v>2225</v>
       </c>
       <c r="I32" s="4">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="J32" s="5">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="K32" s="5">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="L32" s="5">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="M32" s="6">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="N32" t="s">
         <v>13</v>

</xml_diff>